<commit_message>
Officer's questionnaire is Done
</commit_message>
<xml_diff>
--- a/data/Fisheries_Officers_Extension_Officers.xlsx
+++ b/data/Fisheries_Officers_Extension_Officers.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kobo\Shigoley\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rstudio\Clientele\2024\Shigoley-Analysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2244A95-9C44-4E31-A914-2DCC333C8B91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{325E7992-CBC3-4809-831A-D674FB129DF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,9 +22,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="88">
   <si>
-    <t>How many years of experience do you have in working with the fisheries sector?</t>
-  </si>
-  <si>
     <t>Fisheries officer</t>
   </si>
   <si>
@@ -284,6 +281,9 @@
   </si>
   <si>
     <t>interventions success assessment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">experience </t>
   </si>
 </sst>
 </file>
@@ -627,8 +627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="W1" sqref="W1:AF1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -638,737 +638,737 @@
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C1" t="s">
         <v>71</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>72</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>73</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>74</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>75</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>76</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J1" t="s">
         <v>77</v>
       </c>
-      <c r="I1" t="s">
-        <v>50</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" t="s">
         <v>78</v>
       </c>
-      <c r="K1" t="s">
-        <v>6</v>
-      </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>79</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O1" t="s">
         <v>80</v>
       </c>
-      <c r="N1" t="s">
-        <v>8</v>
-      </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q1" t="s">
         <v>81</v>
       </c>
-      <c r="P1" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>82</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>83</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>84</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>85</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>86</v>
-      </c>
-      <c r="V1" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>5</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2" t="s">
         <v>6</v>
       </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2">
-        <v>1</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>7</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="R2" t="s">
+        <v>2</v>
+      </c>
+      <c r="S2" t="s">
         <v>8</v>
       </c>
-      <c r="N2">
-        <v>1</v>
-      </c>
-      <c r="O2">
-        <v>0</v>
-      </c>
-      <c r="P2">
-        <v>0</v>
-      </c>
-      <c r="R2" t="s">
-        <v>3</v>
-      </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
+        <v>2</v>
+      </c>
+      <c r="U2" t="s">
+        <v>2</v>
+      </c>
+      <c r="V2" t="s">
         <v>9</v>
-      </c>
-      <c r="T2" t="s">
-        <v>3</v>
-      </c>
-      <c r="U2" t="s">
-        <v>3</v>
-      </c>
-      <c r="V2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3">
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
         <v>3</v>
       </c>
-      <c r="E3" t="s">
-        <v>4</v>
-      </c>
       <c r="F3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" t="s">
         <v>11</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3" t="s">
+        <v>6</v>
+      </c>
+      <c r="M3" t="s">
         <v>12</v>
       </c>
-      <c r="H3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3">
-        <v>1</v>
-      </c>
-      <c r="L3" t="s">
-        <v>7</v>
-      </c>
-      <c r="M3" t="s">
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>1</v>
+      </c>
+      <c r="R3" t="s">
+        <v>2</v>
+      </c>
+      <c r="S3" t="s">
         <v>13</v>
       </c>
-      <c r="N3">
-        <v>1</v>
-      </c>
-      <c r="O3">
-        <v>0</v>
-      </c>
-      <c r="P3">
-        <v>1</v>
-      </c>
-      <c r="R3" t="s">
-        <v>3</v>
-      </c>
-      <c r="S3" t="s">
+      <c r="T3" t="s">
         <v>14</v>
       </c>
-      <c r="T3" t="s">
+      <c r="U3" t="s">
         <v>15</v>
       </c>
-      <c r="U3" t="s">
+      <c r="V3" t="s">
         <v>16</v>
-      </c>
-      <c r="V3" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B4">
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
         <v>3</v>
       </c>
-      <c r="E4" t="s">
-        <v>4</v>
-      </c>
       <c r="F4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" t="s">
         <v>18</v>
       </c>
-      <c r="G4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4" t="s">
         <v>19</v>
       </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
-      <c r="J4">
-        <v>1</v>
-      </c>
-      <c r="K4">
-        <v>1</v>
-      </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>20</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>1</v>
+      </c>
+      <c r="R4" t="s">
+        <v>2</v>
+      </c>
+      <c r="S4" t="s">
         <v>21</v>
       </c>
-      <c r="N4">
-        <v>0</v>
-      </c>
-      <c r="O4">
-        <v>0</v>
-      </c>
-      <c r="P4">
-        <v>1</v>
-      </c>
-      <c r="R4" t="s">
-        <v>3</v>
-      </c>
-      <c r="S4" t="s">
+      <c r="T4" t="s">
+        <v>2</v>
+      </c>
+      <c r="U4" t="s">
         <v>22</v>
       </c>
-      <c r="T4" t="s">
-        <v>3</v>
-      </c>
-      <c r="U4" t="s">
+      <c r="V4" t="s">
         <v>23</v>
-      </c>
-      <c r="V4" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B5">
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" t="s">
         <v>26</v>
       </c>
-      <c r="F5" t="s">
+      <c r="R5" t="s">
+        <v>2</v>
+      </c>
+      <c r="S5" t="s">
         <v>27</v>
       </c>
-      <c r="R5" t="s">
-        <v>3</v>
-      </c>
-      <c r="S5" t="s">
+      <c r="T5" t="s">
+        <v>2</v>
+      </c>
+      <c r="U5" t="s">
         <v>28</v>
       </c>
-      <c r="T5" t="s">
-        <v>3</v>
-      </c>
-      <c r="U5" t="s">
+      <c r="V5" t="s">
         <v>29</v>
-      </c>
-      <c r="V5" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B6">
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" t="s">
         <v>31</v>
       </c>
-      <c r="E6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6" t="s">
+        <v>19</v>
+      </c>
+      <c r="M6" t="s">
+        <v>7</v>
+      </c>
+      <c r="N6">
+        <v>1</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="R6" t="s">
+        <v>30</v>
+      </c>
+      <c r="S6" t="s">
         <v>32</v>
       </c>
-      <c r="G6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H6" t="s">
-        <v>6</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6">
-        <v>1</v>
-      </c>
-      <c r="L6" t="s">
-        <v>20</v>
-      </c>
-      <c r="M6" t="s">
-        <v>8</v>
-      </c>
-      <c r="N6">
-        <v>1</v>
-      </c>
-      <c r="O6">
-        <v>0</v>
-      </c>
-      <c r="P6">
-        <v>0</v>
-      </c>
-      <c r="R6" t="s">
-        <v>31</v>
-      </c>
-      <c r="S6" t="s">
+      <c r="T6" t="s">
         <v>33</v>
       </c>
-      <c r="T6" t="s">
+      <c r="U6" t="s">
         <v>34</v>
       </c>
-      <c r="U6" t="s">
+      <c r="V6" t="s">
         <v>35</v>
-      </c>
-      <c r="V6" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B7">
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G7" t="s">
+        <v>36</v>
+      </c>
+      <c r="H7" t="s">
+        <v>5</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7" t="s">
+        <v>19</v>
+      </c>
+      <c r="M7" t="s">
+        <v>7</v>
+      </c>
+      <c r="N7">
+        <v>1</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="R7" t="s">
+        <v>2</v>
+      </c>
+      <c r="S7" t="s">
         <v>37</v>
       </c>
-      <c r="H7" t="s">
-        <v>6</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
-      <c r="K7">
-        <v>1</v>
-      </c>
-      <c r="L7" t="s">
-        <v>20</v>
-      </c>
-      <c r="M7" t="s">
-        <v>8</v>
-      </c>
-      <c r="N7">
-        <v>1</v>
-      </c>
-      <c r="O7">
-        <v>0</v>
-      </c>
-      <c r="P7">
-        <v>0</v>
-      </c>
-      <c r="R7" t="s">
-        <v>3</v>
-      </c>
-      <c r="S7" t="s">
+      <c r="T7" t="s">
         <v>38</v>
       </c>
-      <c r="T7" t="s">
+      <c r="U7" t="s">
         <v>39</v>
       </c>
-      <c r="U7" t="s">
+      <c r="V7" t="s">
         <v>40</v>
-      </c>
-      <c r="V7" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B8">
         <v>10</v>
       </c>
       <c r="C8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" t="s">
         <v>42</v>
       </c>
-      <c r="D8" t="s">
-        <v>3</v>
-      </c>
-      <c r="E8" t="s">
-        <v>26</v>
-      </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" t="s">
+        <v>18</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8" t="s">
+        <v>6</v>
+      </c>
+      <c r="M8" t="s">
         <v>43</v>
       </c>
-      <c r="G8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H8" t="s">
-        <v>19</v>
-      </c>
-      <c r="I8">
-        <v>1</v>
-      </c>
-      <c r="J8">
-        <v>1</v>
-      </c>
-      <c r="K8">
-        <v>1</v>
-      </c>
-      <c r="L8" t="s">
-        <v>7</v>
-      </c>
-      <c r="M8" t="s">
+      <c r="N8">
+        <v>1</v>
+      </c>
+      <c r="O8">
+        <v>1</v>
+      </c>
+      <c r="P8">
+        <v>1</v>
+      </c>
+      <c r="R8" t="s">
+        <v>2</v>
+      </c>
+      <c r="S8" t="s">
         <v>44</v>
       </c>
-      <c r="N8">
-        <v>1</v>
-      </c>
-      <c r="O8">
-        <v>1</v>
-      </c>
-      <c r="P8">
-        <v>1</v>
-      </c>
-      <c r="R8" t="s">
-        <v>3</v>
-      </c>
-      <c r="S8" t="s">
+      <c r="T8" t="s">
         <v>45</v>
       </c>
-      <c r="T8" t="s">
+      <c r="U8" t="s">
         <v>46</v>
       </c>
-      <c r="U8" t="s">
+      <c r="V8" t="s">
         <v>47</v>
-      </c>
-      <c r="V8" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B9">
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E9" t="s">
+        <v>48</v>
+      </c>
+      <c r="G9" t="s">
+        <v>4</v>
+      </c>
+      <c r="H9" t="s">
         <v>49</v>
       </c>
-      <c r="G9" t="s">
-        <v>5</v>
-      </c>
-      <c r="H9" t="s">
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9" t="s">
+        <v>19</v>
+      </c>
+      <c r="M9" t="s">
+        <v>7</v>
+      </c>
+      <c r="N9">
+        <v>1</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="R9" t="s">
+        <v>2</v>
+      </c>
+      <c r="S9" t="s">
         <v>50</v>
       </c>
-      <c r="I9">
-        <v>1</v>
-      </c>
-      <c r="J9">
-        <v>0</v>
-      </c>
-      <c r="K9">
-        <v>0</v>
-      </c>
-      <c r="L9" t="s">
-        <v>20</v>
-      </c>
-      <c r="M9" t="s">
-        <v>8</v>
-      </c>
-      <c r="N9">
-        <v>1</v>
-      </c>
-      <c r="O9">
-        <v>0</v>
-      </c>
-      <c r="P9">
-        <v>0</v>
-      </c>
-      <c r="R9" t="s">
-        <v>3</v>
-      </c>
-      <c r="S9" t="s">
+      <c r="T9" t="s">
         <v>51</v>
       </c>
-      <c r="T9" t="s">
+      <c r="U9" t="s">
         <v>52</v>
       </c>
-      <c r="U9" t="s">
+      <c r="V9" t="s">
         <v>53</v>
-      </c>
-      <c r="V9" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B10">
         <v>9</v>
       </c>
       <c r="C10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" t="s">
         <v>55</v>
       </c>
-      <c r="D10" t="s">
-        <v>3</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="G10" t="s">
         <v>4</v>
       </c>
-      <c r="F10" t="s">
+      <c r="H10" t="s">
+        <v>5</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
+      <c r="L10" t="s">
+        <v>6</v>
+      </c>
+      <c r="M10" t="s">
         <v>56</v>
       </c>
-      <c r="G10" t="s">
-        <v>5</v>
-      </c>
-      <c r="H10" t="s">
-        <v>6</v>
-      </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
-      <c r="J10">
-        <v>0</v>
-      </c>
-      <c r="K10">
-        <v>1</v>
-      </c>
-      <c r="L10" t="s">
-        <v>7</v>
-      </c>
-      <c r="M10" t="s">
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10" t="s">
         <v>57</v>
       </c>
-      <c r="N10">
-        <v>0</v>
-      </c>
-      <c r="O10">
-        <v>0</v>
-      </c>
-      <c r="P10">
-        <v>0</v>
-      </c>
-      <c r="Q10" t="s">
+      <c r="R10" t="s">
+        <v>2</v>
+      </c>
+      <c r="S10" t="s">
         <v>58</v>
       </c>
-      <c r="R10" t="s">
-        <v>3</v>
-      </c>
-      <c r="S10" t="s">
+      <c r="T10" t="s">
         <v>59</v>
       </c>
-      <c r="T10" t="s">
+      <c r="U10" t="s">
         <v>60</v>
       </c>
-      <c r="U10" t="s">
+      <c r="V10" t="s">
         <v>61</v>
-      </c>
-      <c r="V10" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B11">
         <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F11" t="s">
+        <v>62</v>
+      </c>
+      <c r="G11" t="s">
+        <v>4</v>
+      </c>
+      <c r="H11" t="s">
         <v>63</v>
       </c>
-      <c r="G11" t="s">
-        <v>5</v>
-      </c>
-      <c r="H11" t="s">
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11" t="s">
+        <v>19</v>
+      </c>
+      <c r="M11" t="s">
+        <v>56</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11" t="s">
         <v>64</v>
       </c>
-      <c r="I11">
-        <v>1</v>
-      </c>
-      <c r="J11">
-        <v>0</v>
-      </c>
-      <c r="K11">
-        <v>1</v>
-      </c>
-      <c r="L11" t="s">
-        <v>20</v>
-      </c>
-      <c r="M11" t="s">
-        <v>57</v>
-      </c>
-      <c r="N11">
-        <v>0</v>
-      </c>
-      <c r="O11">
-        <v>0</v>
-      </c>
-      <c r="P11">
-        <v>0</v>
-      </c>
-      <c r="Q11" t="s">
+      <c r="R11" t="s">
+        <v>2</v>
+      </c>
+      <c r="S11" t="s">
         <v>65</v>
       </c>
-      <c r="R11" t="s">
-        <v>3</v>
-      </c>
-      <c r="S11" t="s">
+      <c r="T11" t="s">
         <v>66</v>
-      </c>
-      <c r="T11" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B12">
         <v>3</v>
       </c>
       <c r="C12" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F12" t="s">
+        <v>67</v>
+      </c>
+      <c r="G12" t="s">
         <v>4</v>
       </c>
-      <c r="F12" t="s">
+      <c r="H12" t="s">
+        <v>5</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12" t="s">
         <v>68</v>
       </c>
-      <c r="G12" t="s">
-        <v>5</v>
-      </c>
-      <c r="H12" t="s">
-        <v>6</v>
-      </c>
-      <c r="I12">
-        <v>0</v>
-      </c>
-      <c r="J12">
-        <v>0</v>
-      </c>
-      <c r="K12">
-        <v>1</v>
-      </c>
-      <c r="L12" t="s">
+      <c r="R12" t="s">
+        <v>30</v>
+      </c>
+      <c r="S12" t="s">
         <v>69</v>
       </c>
-      <c r="R12" t="s">
-        <v>31</v>
-      </c>
-      <c r="S12" t="s">
-        <v>70</v>
-      </c>
       <c r="T12" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="U12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="V12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>